<commit_message>
carga documento e ingreso
</commit_message>
<xml_diff>
--- a/Excel/Carga DB Postgres/Documento - cargado.xlsx
+++ b/Excel/Carga DB Postgres/Documento - cargado.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>url</t>
   </si>
@@ -24,94 +24,97 @@
     <t>idingreso</t>
   </si>
   <si>
-    <t>201711070001INVE</t>
-  </si>
-  <si>
-    <t>201711070002INVE</t>
-  </si>
-  <si>
-    <t>201711070003DNI</t>
-  </si>
-  <si>
-    <t>201711070004LICE</t>
-  </si>
-  <si>
-    <t>201711070005CEDUV</t>
-  </si>
-  <si>
-    <t>201711070006SEGU</t>
-  </si>
-  <si>
-    <t>201711070007VTV</t>
-  </si>
-  <si>
-    <t>201711070008DGAI</t>
-  </si>
-  <si>
-    <t>201711070009DNI</t>
-  </si>
-  <si>
-    <t>201711070010ACTAZ</t>
-  </si>
-  <si>
-    <t>201711070011CEDUV</t>
-  </si>
-  <si>
-    <t>201711070012SEGU</t>
-  </si>
-  <si>
-    <t>201711070013VTV</t>
-  </si>
-  <si>
-    <t>201711070014DGAI</t>
-  </si>
-  <si>
-    <t>201711070015DNI</t>
-  </si>
-  <si>
-    <t>201711070017DGAI</t>
-  </si>
-  <si>
-    <t>201711070018POFI</t>
-  </si>
-  <si>
-    <t>201711070019OFIJU</t>
-  </si>
-  <si>
-    <t>201711070020ACTAE</t>
-  </si>
-  <si>
-    <t>201711070016CEDUT</t>
-  </si>
-  <si>
-    <t>201711070021DISPAN</t>
-  </si>
-  <si>
-    <t>201711070022INFOD</t>
-  </si>
-  <si>
-    <t>201711070023CEDUN</t>
-  </si>
-  <si>
-    <t>201711070024REMI</t>
-  </si>
-  <si>
-    <t>201711070025NOTAC</t>
-  </si>
-  <si>
-    <t>201711070026EXPE</t>
-  </si>
-  <si>
-    <t>201711070027EDIC</t>
-  </si>
-  <si>
-    <t>201711070028SECUP</t>
-  </si>
-  <si>
-    <t>201711070029SECUN</t>
-  </si>
-  <si>
     <t>idtipodocumento</t>
+  </si>
+  <si>
+    <t>2017-11-07_REG-026_INVE</t>
+  </si>
+  <si>
+    <t>2017-11-07_REG-027_INVE</t>
+  </si>
+  <si>
+    <t>2017-11-07_REG-001_DNI</t>
+  </si>
+  <si>
+    <t>2017-11-07_REG-001_LICE</t>
+  </si>
+  <si>
+    <t>2017-11-07_REG-001_CEDUV</t>
+  </si>
+  <si>
+    <t>2017-11-07_REG-001_SEGU</t>
+  </si>
+  <si>
+    <t>2017-11-07_REG-001_VTV</t>
+  </si>
+  <si>
+    <t>2017-11-07_REG-001_DGAI</t>
+  </si>
+  <si>
+    <t>2017-11-07_REG-002_DNI</t>
+  </si>
+  <si>
+    <t>2017-11-07_REG-002_ACTAZ</t>
+  </si>
+  <si>
+    <t>2017-11-07_REG-002_CEDUV</t>
+  </si>
+  <si>
+    <t>2017-11-07_REG-002_SEGU</t>
+  </si>
+  <si>
+    <t>2017-11-07_REG-002_VTV</t>
+  </si>
+  <si>
+    <t>2017-11-07_REG-002_DGAI</t>
+  </si>
+  <si>
+    <t>2017-11-07_REG-121_DNI</t>
+  </si>
+  <si>
+    <t>2017-11-07_REG-121_CEDUT</t>
+  </si>
+  <si>
+    <t>2017-11-07_REG-121_DGAI</t>
+  </si>
+  <si>
+    <t>2017-11-07_REG-121_POFI</t>
+  </si>
+  <si>
+    <t>2017-11-07_REG-122_OFIJU</t>
+  </si>
+  <si>
+    <t>2017-11-07_REG-005_ACTAE</t>
+  </si>
+  <si>
+    <t>2017-11-07_REG-022_DISPAN</t>
+  </si>
+  <si>
+    <t>2017-11-07_REG-022_INFOD</t>
+  </si>
+  <si>
+    <t>2017-11-07_REG-022_CEDUN</t>
+  </si>
+  <si>
+    <t>2017-11-07_REG-022_REMI</t>
+  </si>
+  <si>
+    <t>2017-11-07_REG-022_NOTAC</t>
+  </si>
+  <si>
+    <t>2017-11-07_REG-022_EXPE</t>
+  </si>
+  <si>
+    <t>2017-11-07_REG-022_EDIC</t>
+  </si>
+  <si>
+    <t>2017-11-07_REG-023_SECUP</t>
+  </si>
+  <si>
+    <t>2017-11-07_REG-024_SECUN</t>
+  </si>
+  <si>
+    <t>2017-11-07_REG-025_BOLEC</t>
   </si>
 </sst>
 </file>
@@ -443,10 +446,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -463,12 +466,12 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>31</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2">
         <v>26</v>
@@ -479,7 +482,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3">
         <v>27</v>
@@ -490,7 +493,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -501,7 +504,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -512,7 +515,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -523,7 +526,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -534,7 +537,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -545,7 +548,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -556,7 +559,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B10">
         <v>2</v>
@@ -567,7 +570,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B11">
         <v>2</v>
@@ -578,7 +581,7 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B12">
         <v>2</v>
@@ -589,7 +592,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B13">
         <v>2</v>
@@ -600,7 +603,7 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B14">
         <v>2</v>
@@ -611,7 +614,7 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B15">
         <v>2</v>
@@ -622,7 +625,7 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B16">
         <v>121</v>
@@ -633,7 +636,7 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B17">
         <v>121</v>
@@ -644,7 +647,7 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B18">
         <v>121</v>
@@ -655,7 +658,7 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B19">
         <v>121</v>
@@ -666,7 +669,7 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B20">
         <v>122</v>
@@ -677,7 +680,7 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B21">
         <v>5</v>
@@ -688,7 +691,7 @@
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B22">
         <v>22</v>
@@ -699,7 +702,7 @@
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B23">
         <v>22</v>
@@ -710,7 +713,7 @@
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B24">
         <v>22</v>
@@ -721,7 +724,7 @@
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B25">
         <v>22</v>
@@ -732,7 +735,7 @@
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B26">
         <v>22</v>
@@ -743,7 +746,7 @@
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B27">
         <v>22</v>
@@ -754,7 +757,7 @@
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B28">
         <v>22</v>
@@ -765,7 +768,7 @@
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B29">
         <v>23</v>
@@ -776,13 +779,24 @@
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B30">
         <v>24</v>
       </c>
       <c r="C30">
         <v>21</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" t="s">
+        <v>32</v>
+      </c>
+      <c r="B31">
+        <v>25</v>
+      </c>
+      <c r="C31">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>